<commit_message>
added elements to recommendation
</commit_message>
<xml_diff>
--- a/apps/comparator/res/concept-mappings.xlsx
+++ b/apps/comparator/res/concept-mappings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
   <si>
     <t xml:space="preserve">system</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">bool</t>
   </si>
   <si>
-    <t xml:space="preserve">http://snomed.info/sct</t>
+    <t xml:space="preserve">https://snomed.info/sct</t>
   </si>
   <si>
     <t xml:space="preserve">840539006</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">supine</t>
   </si>
   <si>
-    <t xml:space="preserve">http://snomed.info/sct/</t>
+    <t xml:space="preserve">https://snomed.info/sct/</t>
   </si>
   <si>
     <t xml:space="preserve">40199007</t>
@@ -190,7 +190,7 @@
     <t xml:space="preserve">SnomedCT: Body position finding (finding)</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.cochrane.org/ontologies/pico/</t>
+    <t xml:space="preserve">https://data.cochrane.org/ontologies/pico/</t>
   </si>
   <si>
     <t xml:space="preserve">Dose</t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">SnomedCT: Duration of treatment (qualifier value)</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.cochrane.org/ontologies/core/</t>
+    <t xml:space="preserve">https://data.cochrane.org/ontologies/core/</t>
   </si>
   <si>
     <t xml:space="preserve">Drug</t>
@@ -251,6 +251,78 @@
   </si>
   <si>
     <t xml:space="preserve">Ventilation Finding (finding)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4hp3qg8yn71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition - Respiratory Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86290005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respiratory measure (observable entity) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4hp3pkr3yl3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition - Acute Respiratory Distress Syndrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oxygenation_index_cacl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmHg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67782005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acute respiratory distress syndrome (disorder)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4hp3p86xjp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition - Sepsis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deltaSOFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91302008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sepsis (disorder)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catecholamine-therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catecholamine Therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drug_norepinephrine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">µg/kg/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drug_epinephrine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drug_vasopressin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E/kg/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drug_dobutamine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drug_dopamine</t>
   </si>
 </sst>
 </file>
@@ -383,6 +455,17 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -391,20 +474,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25:D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,7 +933,240 @@
         <v>47</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D33:D37">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$V33=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added OR capabilities to comparator
</commit_message>
<xml_diff>
--- a/apps/comparator/res/concept-mappings.xlsx
+++ b/apps/comparator/res/concept-mappings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="102">
   <si>
     <t xml:space="preserve">system</t>
   </si>
@@ -259,6 +259,9 @@
     <t xml:space="preserve">Condition - Respiratory Rate</t>
   </si>
   <si>
+    <t xml:space="preserve">respiratory_rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">86290005</t>
   </si>
   <si>
@@ -271,7 +274,7 @@
     <t xml:space="preserve">Condition - Acute Respiratory Distress Syndrome</t>
   </si>
   <si>
-    <t xml:space="preserve">oxygenation_index_cacl</t>
+    <t xml:space="preserve">oxygenation_index_calc</t>
   </si>
   <si>
     <t xml:space="preserve">mmHg</t>
@@ -298,10 +301,10 @@
     <t xml:space="preserve">Sepsis (disorder)</t>
   </si>
   <si>
-    <t xml:space="preserve">catecholamine-therapy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catecholamine Therapy</t>
+    <t xml:space="preserve">vasopressor-therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vasopressor Therapy</t>
   </si>
   <si>
     <t xml:space="preserve">drug_norepinephrine</t>
@@ -476,17 +479,17 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.13"/>
   </cols>
   <sheetData>
@@ -943,16 +946,22 @@
       <c r="C27" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="D27" s="0" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,13 +969,13 @@
         <v>9</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>37</v>
@@ -975,7 +984,7 @@
         <v>300</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,13 +992,13 @@
         <v>14</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>37</v>
@@ -998,7 +1007,7 @@
         <v>300</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,13 +1015,13 @@
         <v>9</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>33</v>
@@ -1026,13 +1035,13 @@
         <v>14</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>33</v>
@@ -1046,13 +1055,13 @@
         <v>29</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>37</v>
@@ -1061,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,13 +1078,13 @@
         <v>29</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>37</v>
@@ -1084,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,13 +1101,13 @@
         <v>29</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>37</v>
@@ -1107,7 +1116,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,13 +1124,13 @@
         <v>29</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>37</v>
@@ -1130,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1138,13 +1147,13 @@
         <v>29</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>37</v>
@@ -1153,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>